<commit_message>
update formatting of result files
</commit_message>
<xml_diff>
--- a/experiments/results/results-all-2opt.xlsx
+++ b/experiments/results/results-all-2opt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milena Lengauer\Documents\Studium\Master\Masterarbeit\Auswertungen\Evaluations_Thesis\AllAlgorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAA3620-7DCB-40B6-AB1D-859C284F1590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59144B96-CA0F-4E7C-835A-CF6E62D2D4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Std. Dev. %</t>
-  </si>
-  <si>
     <t>Recovery Rate</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   <si>
     <t>Absolute RR - Std. Dev. %</t>
   </si>
+  <si>
+    <t>Var.Koeff.</t>
+  </si>
 </sst>
 </file>
 
@@ -185,18 +185,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,23 +206,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -514,119 +507,119 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F928C562-0284-4C61-848C-62D414FC9D52}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="I1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="J2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4" t="s">
+      <c r="F3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="G3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="L3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <f>'fast-low'!J3</f>
         <v>7.7994805233393222E-2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <f>'fast-medium'!J3</f>
         <v>0.14334320363239977</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <f>'fast-high'!J3</f>
         <v>0.29162603945674104</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <f>'slow-low'!J3</f>
         <v>5.8293399421018903E-2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="3">
         <f>'slow-medium'!J3</f>
         <v>7.8188644963961343E-2</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="3">
         <f>'slow-high'!J3</f>
         <v>0.12135342541148332</v>
       </c>
@@ -659,30 +652,30 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <f>'fast-low'!J4</f>
         <v>7.108832195176415E-2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <f>'fast-medium'!J4</f>
         <v>0.12852254690355597</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <f>'fast-high'!J4</f>
         <v>0.25454962892765082</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <f>'slow-low'!J4</f>
         <v>5.4770233854636037E-2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <f>'slow-medium'!J4</f>
         <v>7.183802286892349E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="3">
         <f>'slow-high'!J4</f>
         <v>0.11366953766776765</v>
       </c>
@@ -715,30 +708,30 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <f>'fast-low'!J5</f>
         <v>8.4497117883535602E-2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <f>'fast-medium'!J5</f>
         <v>0.1574329219014296</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <f>'fast-high'!J5</f>
         <v>0.34590630082619089</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <f>'slow-low'!J5</f>
         <v>6.1165703674325458E-2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="3">
         <f>'slow-medium'!J5</f>
         <v>8.0938730804191811E-2</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="3">
         <f>'slow-high'!J5</f>
         <v>0.13721843399998016</v>
       </c>
@@ -769,33 +762,33 @@
         <f>'slow-high'!L5</f>
         <v>9.8287003301691267E-2</v>
       </c>
-      <c r="Q6" s="7"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <f>'fast-low'!J6</f>
         <v>0.15524068560006996</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <f>'fast-medium'!J6</f>
         <v>0.37257772335437156</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <f>'fast-high'!J6</f>
         <v>0.85381698218089219</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <f>'slow-low'!J6</f>
         <v>7.2643799231707051E-2</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="3">
         <f>'slow-medium'!J6</f>
         <v>0.1439741185355044</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="3">
         <f>'slow-high'!J6</f>
         <v>0.30231042249359585</v>
       </c>
@@ -828,30 +821,30 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <f>'fast-low'!J7</f>
         <v>7.8318221383716843E-2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <f>'fast-medium'!J7</f>
         <v>0.17092581998833925</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <f>'fast-high'!J7</f>
         <v>0.37362712891259559</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="3">
         <f>'slow-low'!J7</f>
         <v>4.5163552616674596E-2</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="3">
         <f>'slow-medium'!J7</f>
         <v>7.4898578866769094E-2</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="3">
         <f>'slow-high'!J7</f>
         <v>0.13598547888255264</v>
       </c>
@@ -884,30 +877,30 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
         <f>'fast-low'!J8</f>
         <v>7.4049166118656792E-2</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <f>'fast-medium'!J8</f>
         <v>0.13787660307719057</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <f>'fast-high'!J8</f>
         <v>0.2838624221390269</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="3">
         <f>'slow-low'!J8</f>
         <v>4.2977827902188286E-2</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="3">
         <f>'slow-medium'!J8</f>
         <v>6.2897096468341462E-2</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="3">
         <f>'slow-high'!J8</f>
         <v>0.10784854617250898</v>
       </c>
@@ -940,30 +933,30 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <f>'fast-low'!J9</f>
         <v>5.8215428968703554E-2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <f>'fast-medium'!J9</f>
         <v>0.10546375517435662</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="3">
         <f>'fast-high'!J9</f>
         <v>0.23231706224400428</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="3">
         <f>'slow-low'!J9</f>
         <v>3.2502512551258772E-2</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="3">
         <f>'slow-medium'!J9</f>
         <v>4.8588215182909053E-2</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="3">
         <f>'slow-high'!J9</f>
         <v>8.4658689233518894E-2</v>
       </c>
@@ -996,83 +989,83 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="I13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="I13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="J14" s="8" t="s">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="J14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="M15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1468,83 +1461,83 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="I25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="I25" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="J26" s="8" t="s">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="J26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="M27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -1940,83 +1933,83 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="I37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="I37" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="J38" s="8" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="J38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="M39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -2413,30 +2406,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="I37:O37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="I25:O25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="I13:O13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="I13:O13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="I25:O25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="I37:O37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="M38:O38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2447,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,15 +2470,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2510,7 +2503,7 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -2863,15 +2856,15 @@
       <c r="E11">
         <v>0.64491526396344701</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2896,7 +2889,7 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -3249,15 +3242,15 @@
       <c r="E21">
         <v>0.54668237560910005</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="I21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -3282,7 +3275,7 @@
         <v>13</v>
       </c>
       <c r="L22" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -3635,15 +3628,15 @@
       <c r="E31">
         <v>0.56603302089979401</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -3668,7 +3661,7 @@
         <v>13</v>
       </c>
       <c r="L32" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -6930,8 +6923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2456B3A-30FA-4921-9DE9-8470D3985088}">
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6958,15 +6951,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6991,7 +6984,7 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -7344,15 +7337,15 @@
       <c r="E11">
         <v>0.62786840518600096</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -7377,7 +7370,7 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -7730,15 +7723,15 @@
       <c r="E21">
         <v>0.61836526144460502</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="I21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -7763,7 +7756,7 @@
         <v>13</v>
       </c>
       <c r="L22" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -8116,15 +8109,15 @@
       <c r="E31">
         <v>0.60558814076595402</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -8149,7 +8142,7 @@
         <v>13</v>
       </c>
       <c r="L32" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -11411,8 +11404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D04E948-34F1-4E77-B6A3-A610B690F323}">
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11437,15 +11430,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -11470,7 +11463,7 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -11823,15 +11816,15 @@
       <c r="E11">
         <v>0.78708440849577599</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -11856,7 +11849,7 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -12209,15 +12202,15 @@
       <c r="E21">
         <v>0.83690113282533896</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="I21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -12242,7 +12235,7 @@
         <v>13</v>
       </c>
       <c r="L22" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -12595,15 +12588,15 @@
       <c r="E31">
         <v>0.86103855708135402</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -12628,7 +12621,7 @@
         <v>13</v>
       </c>
       <c r="L32" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -15887,8 +15880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F9A15D-8B11-4DEC-B61C-69A0E6587E9C}">
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15913,15 +15906,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -15946,7 +15939,7 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -16299,15 +16292,15 @@
       <c r="E11">
         <v>0.80800427128671404</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -16332,7 +16325,7 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -16685,15 +16678,15 @@
       <c r="E21">
         <v>0.79016534472560995</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="I21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -16718,7 +16711,7 @@
         <v>13</v>
       </c>
       <c r="L22" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -17071,15 +17064,15 @@
       <c r="E31">
         <v>0.83606324160679102</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -17104,7 +17097,7 @@
         <v>13</v>
       </c>
       <c r="L32" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -20363,8 +20356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F6514D-47FE-4B29-9BDD-A95D7DABE5FB}">
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142:E211"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20389,15 +20382,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -20422,7 +20415,7 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -20775,15 +20768,15 @@
       <c r="E11">
         <v>0.87686111296365299</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -20808,7 +20801,7 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -21161,15 +21154,15 @@
       <c r="E21">
         <v>0.89867421558331695</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="I21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -21194,7 +21187,7 @@
         <v>13</v>
       </c>
       <c r="L22" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -21547,15 +21540,15 @@
       <c r="E31">
         <v>0.90214911456958602</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -21580,7 +21573,7 @@
         <v>13</v>
       </c>
       <c r="L32" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -24839,8 +24832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399D309C-A375-44B0-ACAF-D01517DCE955}">
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24868,15 +24861,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -24901,7 +24894,7 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -25254,15 +25247,15 @@
       <c r="E11">
         <v>0.91539959268482696</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -25287,7 +25280,7 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -25640,15 +25633,15 @@
       <c r="E21">
         <v>0.93075985511308501</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="I21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -25673,7 +25666,7 @@
         <v>13</v>
       </c>
       <c r="L22" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -26026,15 +26019,15 @@
       <c r="E31">
         <v>0.92878364383743695</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -26059,7 +26052,7 @@
         <v>13</v>
       </c>
       <c r="L32" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>

</xml_diff>